<commit_message>
red, green and blue stacking
</commit_message>
<xml_diff>
--- a/Cartesian Co-ordinates for Dobot.xlsx
+++ b/Cartesian Co-ordinates for Dobot.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\McDou\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\McDou\OneDrive - University of Greenwich\Year 4\Year 4 - Digital and Embedded Electronic Systems\Dobot Github\ELEE-1144-M02-2025-26-Dobot-Arm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C9183432-363A-4F43-821B-FC100C4DE5B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45C97DA6-5279-41DF-8357-66C77758036D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="11890" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{E45B4B61-985F-4334-B999-D24102406AEE}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="50">
   <si>
     <t>Cartesian: 201.78 -147.60 -53.77 -36.19 Polar: -36.19 57.77 58.82 -0.00</t>
   </si>
@@ -130,9 +130,6 @@
     <t>Cartesian: 72.60 -259.71 67.63 -102.58</t>
   </si>
   <si>
-    <t>redStorage LOW</t>
-  </si>
-  <si>
     <t>Cartesian: 76.73 -228.93 -54.06 -99.67</t>
   </si>
   <si>
@@ -176,6 +173,21 @@
   </si>
   <si>
     <t>Cartesian: 204.90 -167.45 5.04 -67.45</t>
+  </si>
+  <si>
+    <t>redStorage space1</t>
+  </si>
+  <si>
+    <t>redStorage space2</t>
+  </si>
+  <si>
+    <t>redStorage space3</t>
+  </si>
+  <si>
+    <t>Cartesian: 82.73, -228.93, -22.06, -99.67</t>
+  </si>
+  <si>
+    <t>Cartesian: 85.73, -228.93, 10, -99.67</t>
   </si>
 </sst>
 </file>
@@ -657,10 +669,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C3A83A5-8972-447A-AD74-6DBEBE09A2EC}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -673,7 +685,7 @@
         <v>20</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -681,7 +693,7 @@
         <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -726,58 +738,74 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="B10" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>44</v>
+      </c>
+      <c r="B16" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated & Corrected Cartesian Coordinates
</commit_message>
<xml_diff>
--- a/Cartesian Co-ordinates for Dobot.xlsx
+++ b/Cartesian Co-ordinates for Dobot.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\McDou\OneDrive - University of Greenwich\Year 4\Year 4 - Digital and Embedded Electronic Systems\Dobot Github\ELEE-1144-M02-2025-26-Dobot-Arm\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\weshu\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45C97DA6-5279-41DF-8357-66C77758036D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6385A22-29A3-4A4B-AA99-32F0BA9DA0D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="11890" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{E45B4B61-985F-4334-B999-D24102406AEE}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" activeTab="2" xr2:uid="{E45B4B61-985F-4334-B999-D24102406AEE}"/>
   </bookViews>
   <sheets>
     <sheet name="RedStorage - Attempt 1#" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="61">
   <si>
     <t>Cartesian: 201.78 -147.60 -53.77 -36.19 Polar: -36.19 57.77 58.82 -0.00</t>
   </si>
@@ -106,24 +106,9 @@
     <t>blueStorage HIGH</t>
   </si>
   <si>
-    <t>Cartesian: 185.13 -136.87 65.37 -64.68</t>
-  </si>
-  <si>
-    <t>blueStorage LOW</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Cartesian: 180.82 -125.47 -53.28 -62.96</t>
-  </si>
-  <si>
     <t>greenStorage HIGH</t>
   </si>
   <si>
-    <t>Cartesian: 126.19 -201.51 84.49 -86.15</t>
-  </si>
-  <si>
-    <t>greenStorage LOW</t>
-  </si>
-  <si>
     <t>redStorage HIGH</t>
   </si>
   <si>
@@ -139,9 +124,6 @@
     <t>retrieval HIGH</t>
   </si>
   <si>
-    <t>pIckUp HIGH</t>
-  </si>
-  <si>
     <t>pickUp LOW</t>
   </si>
   <si>
@@ -188,16 +170,99 @@
   </si>
   <si>
     <t>Cartesian: 85.73, -228.93, 10, -99.67</t>
+  </si>
+  <si>
+    <t>greenStorage space1</t>
+  </si>
+  <si>
+    <t>Coordinates</t>
+  </si>
+  <si>
+    <t>Point</t>
+  </si>
+  <si>
+    <t>greenStorage space2</t>
+  </si>
+  <si>
+    <t>greenStorage space3</t>
+  </si>
+  <si>
+    <t>blueStorage space1</t>
+  </si>
+  <si>
+    <t>blueStorage space2</t>
+  </si>
+  <si>
+    <t>blueStorage space3</t>
+  </si>
+  <si>
+    <t>Cartesian: 130.25, -176.69, -54.12, -81.80</t>
+  </si>
+  <si>
+    <t>Cartesian:  130.25, -176.69, 81.42, -81.14</t>
+  </si>
+  <si>
+    <t>Cartesian: 130.25, -176.69, -22.12, -81.80</t>
+  </si>
+  <si>
+    <t>Cartesian: 130.25, -176.69, 10, -81.80</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cartesian: 180.82, -125.47, -53.28, -62.96</t>
+  </si>
+  <si>
+    <t>Cartesian: 185.13, -136.87, 65.37, -64.68</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cartesian: 180.82, -125.47, -22.28, -62.96</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cartesian: 180.82, -125.47, 10.00, -64.68</t>
+  </si>
+  <si>
+    <t>pickUp HIGH</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="3" tint="0.499984740745262"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -211,7 +276,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -219,12 +284,42 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -565,9 +660,9 @@
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -575,7 +670,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -583,7 +678,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -591,7 +686,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -612,9 +707,9 @@
       <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -622,7 +717,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -630,7 +725,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -638,7 +733,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -646,7 +741,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -654,7 +749,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -669,143 +764,183 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C3A83A5-8972-447A-AD74-6DBEBE09A2EC}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="B2:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23:C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.7265625" customWidth="1"/>
+    <col min="2" max="3" width="38.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C3" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B5" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B6" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B7" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B8" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B9" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B10" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B11" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B12" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B15" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B16" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B17" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B18" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B19" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B9" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>49</v>
-      </c>
-      <c r="B10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B20" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B21" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C21" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B22" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C22" s="2" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>39</v>
-      </c>
-      <c r="B14" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>42</v>
-      </c>
-      <c r="B15" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>44</v>
-      </c>
-      <c r="B16" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>